<commit_message>
Updated pick up script
</commit_message>
<xml_diff>
--- a/SelTestNG_DD/TestData/TestDataFile - Copy.xlsx
+++ b/SelTestNG_DD/TestData/TestDataFile - Copy.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Item</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Zip Code</t>
-  </si>
-  <si>
-    <t>Ship to address</t>
   </si>
   <si>
     <t>Pick up at store</t>
@@ -430,7 +427,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A2" sqref="A2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,8 +479,12 @@
       <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="3">
+        <v>558</v>
+      </c>
+      <c r="F2" s="3">
+        <v>18052</v>
+      </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
@@ -500,14 +501,18 @@
       <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="3">
+        <v>558</v>
+      </c>
+      <c r="F3" s="3">
+        <v>18052</v>
+      </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3">
         <v>10789537</v>
@@ -516,13 +521,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3">
-        <v>558</v>
+        <v>2013</v>
       </c>
       <c r="F4" s="3">
-        <v>18052</v>
+        <v>84107</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -538,7 +543,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3">
         <v>558</v>
@@ -560,7 +565,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3">
         <v>83</v>
@@ -582,7 +587,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="3">
         <v>83</v>
@@ -604,7 +609,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="3">
         <v>83</v>

</xml_diff>